<commit_message>
finish Task 6: R-type Instructions, not pass
</commit_message>
<xml_diff>
--- a/[61C SP22] Project 3B ROM Control Logic.xlsx
+++ b/[61C SP22] Project 3B ROM Control Logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\c_c++\cs61c\sp22-proj3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8010A2BB-DB2A-4DD7-A262-237B9ABF4BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FDA825-8858-4CE9-9C50-907B37B96768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control Logic for ROM" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="117">
   <si>
     <t>MAKE A COPY OF THIS SHEET</t>
   </si>
@@ -368,9 +368,6 @@
   </si>
   <si>
     <t>S</t>
-  </si>
-  <si>
-    <t>0b0100011</t>
   </si>
   <si>
     <t>sh rs2, offset(rs1)</t>
@@ -482,6 +479,30 @@
   </si>
   <si>
     <t>0111</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>1100</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>1011</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>0b0100011</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -719,10 +740,26 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,22 +773,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -981,11 +1002,11 @@
   </sheetPr>
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1001,61 +1022,61 @@
     <col min="18" max="23" width="12.6328125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:23" ht="14" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="29" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="36"/>
       <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="32" t="s">
+      <c r="Q1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" s="28"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+    </row>
+    <row r="2" spans="1:23" ht="14" x14ac:dyDescent="0.3">
+      <c r="A2" s="30"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="36"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -1065,7 +1086,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1181,10 +1202,10 @@
       <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="29" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -1201,37 +1222,53 @@
         <f t="shared" ref="G5:G40" si="0">V5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
+      <c r="H5" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J5" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N5" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P5" s="11" t="str">
         <f t="shared" ref="P5:P40" si="1">CONCATENATE(U5,T5)</f>
-        <v>0000</v>
+        <v>1001</v>
       </c>
       <c r="Q5" s="12" t="str">
         <f t="shared" ref="Q5:Q40" si="2">TEXT(CONCATENATE(O5, N5, M5, L5, K5, J5, I5, H5), "0000000000000000")</f>
-        <v/>
+        <v>0001000000000001</v>
       </c>
       <c r="R5" s="12" t="str">
         <f t="shared" ref="R5:R40" si="3">RIGHT(Q5,8)</f>
-        <v/>
+        <v>00000001</v>
       </c>
       <c r="S5" s="12" t="str">
         <f t="shared" ref="S5:S40" si="4">LEFT(Q5,8)</f>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T5" s="12" t="str">
         <f t="shared" ref="T5:U5" si="5">BIN2HEX(R5,2)</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="U5" s="13" t="str">
         <f t="shared" si="5"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V5" s="12">
         <v>0</v>
@@ -1245,8 +1282,8 @@
       <c r="A6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="17" t="s">
         <v>36</v>
       </c>
@@ -1261,37 +1298,53 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="H6" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P6" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1401</v>
       </c>
       <c r="Q6" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001010000000001</v>
       </c>
       <c r="R6" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000001</v>
       </c>
       <c r="S6" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010100</v>
       </c>
       <c r="T6" s="12" t="str">
         <f t="shared" ref="T6:U6" si="7">BIN2HEX(R6,2)</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="U6" s="13" t="str">
         <f t="shared" si="7"/>
-        <v>00</v>
+        <v>14</v>
       </c>
       <c r="V6" s="12">
         <v>1</v>
@@ -1305,8 +1358,8 @@
       <c r="A7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="17" t="s">
         <v>36</v>
       </c>
@@ -1321,37 +1374,53 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="H7" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P7" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1601</v>
       </c>
       <c r="Q7" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001011000000001</v>
       </c>
       <c r="R7" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000001</v>
       </c>
       <c r="S7" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010110</v>
       </c>
       <c r="T7" s="12" t="str">
         <f t="shared" ref="T7:U7" si="8">BIN2HEX(R7,2)</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="U7" s="13" t="str">
         <f t="shared" si="8"/>
-        <v>00</v>
+        <v>16</v>
       </c>
       <c r="V7" s="12">
         <v>2</v>
@@ -1365,8 +1434,8 @@
       <c r="A8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="17" t="s">
         <v>43</v>
       </c>
@@ -1381,37 +1450,53 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="H8" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="N8" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O8" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P8" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1081</v>
       </c>
       <c r="Q8" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000010000001</v>
       </c>
       <c r="R8" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10000001</v>
       </c>
       <c r="S8" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T8" s="12" t="str">
         <f t="shared" ref="T8:U8" si="9">BIN2HEX(R8,2)</f>
-        <v>00</v>
+        <v>81</v>
       </c>
       <c r="U8" s="13" t="str">
         <f t="shared" si="9"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V8" s="12">
         <v>3</v>
@@ -1425,8 +1510,8 @@
       <c r="A9" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="20" t="s">
         <v>43</v>
       </c>
@@ -1441,37 +1526,53 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
+      <c r="H9" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L9" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M9" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="N9" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O9" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P9" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1481</v>
       </c>
       <c r="Q9" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001010010000001</v>
       </c>
       <c r="R9" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10000001</v>
       </c>
       <c r="S9" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010100</v>
       </c>
       <c r="T9" s="12" t="str">
         <f t="shared" ref="T9:U9" si="10">BIN2HEX(R9,2)</f>
-        <v>00</v>
+        <v>81</v>
       </c>
       <c r="U9" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>00</v>
+        <v>14</v>
       </c>
       <c r="V9" s="12">
         <v>4</v>
@@ -1485,8 +1586,8 @@
       <c r="A10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="17" t="s">
         <v>46</v>
       </c>
@@ -1501,37 +1602,53 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
+      <c r="H10" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="N10" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P10" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1581</v>
       </c>
       <c r="Q10" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001010110000001</v>
       </c>
       <c r="R10" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10000001</v>
       </c>
       <c r="S10" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010101</v>
       </c>
       <c r="T10" s="12" t="str">
         <f t="shared" ref="T10:U10" si="11">BIN2HEX(R10,2)</f>
-        <v>00</v>
+        <v>81</v>
       </c>
       <c r="U10" s="13" t="str">
         <f t="shared" si="11"/>
-        <v>00</v>
+        <v>15</v>
       </c>
       <c r="V10" s="12">
         <v>5</v>
@@ -1545,8 +1662,8 @@
       <c r="A11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="17" t="s">
         <v>48</v>
       </c>
@@ -1561,37 +1678,53 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
+      <c r="H11" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L11" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M11" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="N11" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O11" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P11" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1101</v>
       </c>
       <c r="Q11" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000100000001</v>
       </c>
       <c r="R11" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000001</v>
       </c>
       <c r="S11" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010001</v>
       </c>
       <c r="T11" s="12" t="str">
         <f t="shared" ref="T11:U11" si="12">BIN2HEX(R11,2)</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="U11" s="13" t="str">
         <f t="shared" si="12"/>
-        <v>00</v>
+        <v>11</v>
       </c>
       <c r="V11" s="12">
         <v>6</v>
@@ -1605,8 +1738,8 @@
       <c r="A12" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="17" t="s">
         <v>50</v>
       </c>
@@ -1621,37 +1754,53 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
+      <c r="H12" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K12" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="N12" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O12" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P12" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1201</v>
       </c>
       <c r="Q12" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001001000000001</v>
       </c>
       <c r="R12" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000001</v>
       </c>
       <c r="S12" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010010</v>
       </c>
       <c r="T12" s="12" t="str">
         <f t="shared" ref="T12:U12" si="13">BIN2HEX(R12,2)</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="U12" s="13" t="str">
         <f t="shared" si="13"/>
-        <v>00</v>
+        <v>12</v>
       </c>
       <c r="V12" s="12">
         <v>7</v>
@@ -1665,8 +1814,8 @@
       <c r="A13" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="17" t="s">
         <v>52</v>
       </c>
@@ -1681,37 +1830,53 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
+      <c r="H13" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K13" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M13" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O13" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P13" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1281</v>
       </c>
       <c r="Q13" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001001010000001</v>
       </c>
       <c r="R13" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10000001</v>
       </c>
       <c r="S13" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010010</v>
       </c>
       <c r="T13" s="12" t="str">
         <f t="shared" ref="T13:U13" si="14">BIN2HEX(R13,2)</f>
-        <v>00</v>
+        <v>81</v>
       </c>
       <c r="U13" s="13" t="str">
         <f t="shared" si="14"/>
-        <v>00</v>
+        <v>12</v>
       </c>
       <c r="V13" s="12">
         <v>8</v>
@@ -1725,8 +1890,8 @@
       <c r="A14" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="17" t="s">
         <v>52</v>
       </c>
@@ -1741,37 +1906,53 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
+      <c r="H14" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K14" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L14" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M14" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="N14" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O14" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P14" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1681</v>
       </c>
       <c r="Q14" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001011010000001</v>
       </c>
       <c r="R14" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10000001</v>
       </c>
       <c r="S14" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010110</v>
       </c>
       <c r="T14" s="12" t="str">
         <f t="shared" ref="T14:U14" si="15">BIN2HEX(R14,2)</f>
-        <v>00</v>
+        <v>81</v>
       </c>
       <c r="U14" s="13" t="str">
         <f t="shared" si="15"/>
-        <v>00</v>
+        <v>16</v>
       </c>
       <c r="V14" s="12">
         <v>9</v>
@@ -1785,8 +1966,8 @@
       <c r="A15" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="17" t="s">
         <v>55</v>
       </c>
@@ -1801,37 +1982,53 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
+      <c r="H15" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M15" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="N15" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O15" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P15" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1301</v>
       </c>
       <c r="Q15" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001001100000001</v>
       </c>
       <c r="R15" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>00000001</v>
       </c>
       <c r="S15" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010011</v>
       </c>
       <c r="T15" s="12" t="str">
         <f t="shared" ref="T15:U15" si="16">BIN2HEX(R15,2)</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="U15" s="13" t="str">
         <f t="shared" si="16"/>
-        <v>00</v>
+        <v>13</v>
       </c>
       <c r="V15" s="12">
         <v>10</v>
@@ -1845,8 +2042,8 @@
       <c r="A16" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="17" t="s">
         <v>57</v>
       </c>
@@ -1861,37 +2058,53 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
+      <c r="H16" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J16" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="N16" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O16" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P16" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1381</v>
       </c>
       <c r="Q16" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001001110000001</v>
       </c>
       <c r="R16" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>10000001</v>
       </c>
       <c r="S16" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010011</v>
       </c>
       <c r="T16" s="12" t="str">
         <f t="shared" ref="T16:U16" si="17">BIN2HEX(R16,2)</f>
-        <v>00</v>
+        <v>81</v>
       </c>
       <c r="U16" s="13" t="str">
         <f t="shared" si="17"/>
-        <v>00</v>
+        <v>13</v>
       </c>
       <c r="V16" s="12">
         <v>11</v>
@@ -1905,11 +2118,11 @@
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="37" t="s">
-        <v>99</v>
+      <c r="C17" s="32" t="s">
+        <v>98</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>36</v>
@@ -1967,8 +2180,8 @@
       <c r="A18" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="20" t="s">
         <v>43</v>
       </c>
@@ -2025,8 +2238,8 @@
       <c r="A19" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="17" t="s">
         <v>48</v>
       </c>
@@ -2083,8 +2296,8 @@
       <c r="A20" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="36" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="33" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="17" t="s">
@@ -2159,8 +2372,8 @@
       <c r="A21" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="20" t="s">
         <v>43</v>
       </c>
@@ -2175,29 +2388,29 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="H21" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I21" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="J21" s="39" t="s">
+      <c r="H21" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K21" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L21" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M21" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="N21" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O21" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="K21" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="L21" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="M21" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="N21" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="O21" s="39" t="s">
-        <v>103</v>
       </c>
       <c r="P21" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2235,8 +2448,8 @@
       <c r="A22" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="17" t="s">
         <v>48</v>
       </c>
@@ -2249,29 +2462,29 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="H22" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I22" s="39" t="s">
+      <c r="H22" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K22" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L22" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M22" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="J22" s="39" t="s">
+      <c r="N22" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O22" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="K22" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="L22" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="M22" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="N22" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="O22" s="39" t="s">
-        <v>103</v>
       </c>
       <c r="P22" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2309,8 +2522,8 @@
       <c r="A23" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="20" t="s">
         <v>50</v>
       </c>
@@ -2323,29 +2536,29 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="H23" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I23" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="J23" s="39" t="s">
+      <c r="H23" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K23" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L23" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M23" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="N23" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O23" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="K23" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="L23" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="M23" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="N23" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="O23" s="39" t="s">
-        <v>103</v>
       </c>
       <c r="P23" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2383,8 +2596,8 @@
       <c r="A24" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="17" t="s">
         <v>52</v>
       </c>
@@ -2399,29 +2612,29 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="H24" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I24" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="J24" s="39" t="s">
+      <c r="H24" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K24" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L24" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M24" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="N24" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O24" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="K24" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="L24" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="M24" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="N24" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="O24" s="39" t="s">
-        <v>103</v>
       </c>
       <c r="P24" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2459,13 +2672,13 @@
       <c r="A25" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
       <c r="D25" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="38" t="s">
-        <v>100</v>
+      <c r="E25" s="27" t="s">
+        <v>99</v>
       </c>
       <c r="F25" s="17" t="str">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("CONCATENATE(""0b"", TO_TEXT(W25))"),"0b010100")</f>
@@ -2475,29 +2688,29 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H25" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I25" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="J25" s="39" t="s">
+      <c r="H25" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J25" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K25" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M25" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="N25" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O25" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="K25" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="L25" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="M25" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="N25" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="O25" s="39" t="s">
-        <v>103</v>
       </c>
       <c r="P25" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2535,8 +2748,8 @@
       <c r="A26" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="17" t="s">
         <v>55</v>
       </c>
@@ -2549,29 +2762,29 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="H26" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="J26" s="39" t="s">
+      <c r="H26" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J26" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K26" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L26" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M26" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="N26" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O26" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="K26" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="L26" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="M26" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="N26" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="O26" s="39" t="s">
-        <v>103</v>
       </c>
       <c r="P26" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2609,8 +2822,8 @@
       <c r="A27" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="17" t="s">
         <v>57</v>
       </c>
@@ -2623,29 +2836,29 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="H27" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="I27" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="J27" s="39" t="s">
+      <c r="H27" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J27" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K27" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L27" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M27" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="N27" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O27" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="K27" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="L27" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="M27" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="N27" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="O27" s="39" t="s">
-        <v>103</v>
       </c>
       <c r="P27" s="11" t="str">
         <f t="shared" si="1"/>
@@ -2683,11 +2896,11 @@
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="36" t="s">
-        <v>78</v>
+      <c r="C28" s="32" t="s">
+        <v>116</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>36</v>
@@ -2743,10 +2956,10 @@
     </row>
     <row r="29" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+        <v>78</v>
+      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="20" t="s">
         <v>43</v>
       </c>
@@ -2801,10 +3014,10 @@
     </row>
     <row r="30" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+        <v>79</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
       <c r="D30" s="17" t="s">
         <v>48</v>
       </c>
@@ -2859,13 +3072,13 @@
     </row>
     <row r="31" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="C31" s="33" t="s">
         <v>82</v>
-      </c>
-      <c r="C31" s="36" t="s">
-        <v>83</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>36</v>
@@ -2921,10 +3134,10 @@
     </row>
     <row r="32" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+        <v>83</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
       <c r="D32" s="20" t="s">
         <v>43</v>
       </c>
@@ -2979,10 +3192,10 @@
     </row>
     <row r="33" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+        <v>84</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="20" t="s">
         <v>50</v>
       </c>
@@ -3037,10 +3250,10 @@
     </row>
     <row r="34" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+        <v>85</v>
+      </c>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
       <c r="D34" s="17" t="s">
         <v>52</v>
       </c>
@@ -3095,10 +3308,10 @@
     </row>
     <row r="35" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
+        <v>86</v>
+      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
       <c r="D35" s="17" t="s">
         <v>55</v>
       </c>
@@ -3153,10 +3366,10 @@
     </row>
     <row r="36" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
+        <v>87</v>
+      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
       <c r="D36" s="17" t="s">
         <v>57</v>
       </c>
@@ -3211,13 +3424,13 @@
     </row>
     <row r="37" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="C37" s="25" t="s">
         <v>90</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>91</v>
       </c>
       <c r="D37" s="26"/>
       <c r="E37" s="22"/>
@@ -3271,11 +3484,11 @@
     </row>
     <row r="38" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="30"/>
+      <c r="C38" s="25" t="s">
         <v>92</v>
-      </c>
-      <c r="B38" s="28"/>
-      <c r="C38" s="25" t="s">
-        <v>93</v>
       </c>
       <c r="D38" s="26"/>
       <c r="E38" s="22"/>
@@ -3329,13 +3542,13 @@
     </row>
     <row r="39" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>96</v>
       </c>
       <c r="D39" s="26"/>
       <c r="E39" s="22"/>
@@ -3389,13 +3602,13 @@
     </row>
     <row r="40" spans="1:23" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>36</v>
@@ -3451,6 +3664,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="H2:O2"/>
     <mergeCell ref="C5:C16"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="B37:B38"/>
@@ -3461,12 +3680,6 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="C31:C36"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="H2:O2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="A1:A2">

</xml_diff>

<commit_message>
pass Task 7: B-type Instructions
</commit_message>
<xml_diff>
--- a/[61C SP22] Project 3B ROM Control Logic.xlsx
+++ b/[61C SP22] Project 3B ROM Control Logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\c_c++\cs61c\sp22-proj3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FDA825-8858-4CE9-9C50-907B37B96768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3655F5BE-6EB4-46E6-97A3-DDC9E14806D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control Logic for ROM" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="118">
   <si>
     <t>MAKE A COPY OF THIS SHEET</t>
   </si>
@@ -503,6 +503,10 @@
   </si>
   <si>
     <t>0b0100011</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -744,22 +748,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -772,6 +764,18 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1002,11 +1006,11 @@
   </sheetPr>
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20:C27"/>
+      <selection pane="bottomRight" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1023,20 +1027,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="35" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="33" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="30"/>
@@ -1045,11 +1049,11 @@
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
-      <c r="O1" s="36"/>
+      <c r="O1" s="32"/>
       <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="38" t="s">
+      <c r="Q1" s="34" t="s">
         <v>5</v>
       </c>
       <c r="R1" s="30"/>
@@ -1067,7 +1071,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="35" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="30"/>
@@ -1076,7 +1080,7 @@
       <c r="L2" s="30"/>
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
-      <c r="O2" s="36"/>
+      <c r="O2" s="32"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -1202,10 +1206,10 @@
       <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="36" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -2118,10 +2122,10 @@
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="38" t="s">
         <v>98</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -2297,7 +2301,7 @@
         <v>62</v>
       </c>
       <c r="B20" s="30"/>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="39" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="17" t="s">
@@ -2896,10 +2900,10 @@
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="38" t="s">
         <v>116</v>
       </c>
       <c r="D28" s="17" t="s">
@@ -3074,10 +3078,10 @@
       <c r="A31" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="33" t="s">
+      <c r="C31" s="39" t="s">
         <v>82</v>
       </c>
       <c r="D31" s="17" t="s">
@@ -3092,37 +3096,53 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
+      <c r="H31" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="J31" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K31" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L31" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M31" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N31" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O31" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P31" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1064</v>
       </c>
       <c r="Q31" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000001100100</v>
       </c>
       <c r="R31" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100100</v>
       </c>
       <c r="S31" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T31" s="12" t="str">
         <f t="shared" ref="T31:U31" si="32">BIN2HEX(R31,2)</f>
-        <v>00</v>
+        <v>64</v>
       </c>
       <c r="U31" s="13" t="str">
         <f t="shared" si="32"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V31" s="12">
         <v>26</v>
@@ -3150,37 +3170,53 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
+      <c r="H32" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="J32" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K32" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L32" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M32" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N32" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O32" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P32" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1064</v>
       </c>
       <c r="Q32" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000001100100</v>
       </c>
       <c r="R32" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100100</v>
       </c>
       <c r="S32" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T32" s="12" t="str">
         <f t="shared" ref="T32:U32" si="33">BIN2HEX(R32,2)</f>
-        <v>00</v>
+        <v>64</v>
       </c>
       <c r="U32" s="13" t="str">
         <f t="shared" si="33"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V32" s="12">
         <v>27</v>
@@ -3208,37 +3244,53 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
+      <c r="H33" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="J33" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L33" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M33" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N33" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O33" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P33" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1064</v>
       </c>
       <c r="Q33" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000001100100</v>
       </c>
       <c r="R33" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100100</v>
       </c>
       <c r="S33" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T33" s="12" t="str">
         <f t="shared" ref="T33:U33" si="34">BIN2HEX(R33,2)</f>
-        <v>00</v>
+        <v>64</v>
       </c>
       <c r="U33" s="13" t="str">
         <f t="shared" si="34"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V33" s="12">
         <v>28</v>
@@ -3266,37 +3318,53 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
+      <c r="H34" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I34" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="J34" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K34" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L34" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M34" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N34" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O34" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P34" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1064</v>
       </c>
       <c r="Q34" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000001100100</v>
       </c>
       <c r="R34" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01100100</v>
       </c>
       <c r="S34" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T34" s="12" t="str">
         <f t="shared" ref="T34:U34" si="35">BIN2HEX(R34,2)</f>
-        <v>00</v>
+        <v>64</v>
       </c>
       <c r="U34" s="13" t="str">
         <f t="shared" si="35"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V34" s="12">
         <v>29</v>
@@ -3324,37 +3392,53 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
+      <c r="H35" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="J35" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="K35" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L35" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M35" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N35" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O35" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P35" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1074</v>
       </c>
       <c r="Q35" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000001110100</v>
       </c>
       <c r="R35" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01110100</v>
       </c>
       <c r="S35" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T35" s="12" t="str">
         <f t="shared" ref="T35:U35" si="36">BIN2HEX(R35,2)</f>
-        <v>00</v>
+        <v>74</v>
       </c>
       <c r="U35" s="13" t="str">
         <f t="shared" si="36"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V35" s="12">
         <v>30</v>
@@ -3382,37 +3466,53 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
+      <c r="H36" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I36" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="J36" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="K36" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L36" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M36" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N36" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O36" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="P36" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1074</v>
       </c>
       <c r="Q36" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001000001110100</v>
       </c>
       <c r="R36" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01110100</v>
       </c>
       <c r="S36" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00010000</v>
       </c>
       <c r="T36" s="12" t="str">
         <f t="shared" ref="T36:U36" si="37">BIN2HEX(R36,2)</f>
-        <v>00</v>
+        <v>74</v>
       </c>
       <c r="U36" s="13" t="str">
         <f t="shared" si="37"/>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="V36" s="12">
         <v>31</v>
@@ -3426,7 +3526,7 @@
       <c r="A37" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="37" t="s">
         <v>89</v>
       </c>
       <c r="C37" s="25" t="s">
@@ -3664,12 +3764,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="H2:O2"/>
     <mergeCell ref="C5:C16"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="B37:B38"/>
@@ -3680,6 +3774,12 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="C31:C36"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="H2:O2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="A1:A2">

</xml_diff>

<commit_message>
finish Task 8.4: Control Logic, has a bug which might be caused by https://github.com/DryLichen/cs61csp22/blob/main/proj3/cpu/partial-store.circ
</commit_message>
<xml_diff>
--- a/[61C SP22] Project 3B ROM Control Logic.xlsx
+++ b/[61C SP22] Project 3B ROM Control Logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\c_c++\cs61c\sp22-proj3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3655F5BE-6EB4-46E6-97A3-DDC9E14806D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5392BA3D-914D-45CD-B4F3-7367D5B1022D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control Logic for ROM" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="120">
   <si>
     <t>MAKE A COPY OF THIS SHEET</t>
   </si>
@@ -507,6 +507,14 @@
   </si>
   <si>
     <t>010</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>00</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -748,10 +756,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -764,18 +784,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1007,10 +1015,10 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J29" sqref="J29"/>
+      <selection pane="bottomRight" activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1027,20 +1035,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="14" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="37" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="30"/>
@@ -1049,11 +1057,11 @@
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
-      <c r="O1" s="32"/>
+      <c r="O1" s="36"/>
       <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="38" t="s">
         <v>5</v>
       </c>
       <c r="R1" s="30"/>
@@ -1071,7 +1079,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="1"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="39" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="30"/>
@@ -1080,7 +1088,7 @@
       <c r="L2" s="30"/>
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
-      <c r="O2" s="32"/>
+      <c r="O2" s="36"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -1206,10 +1214,10 @@
       <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="29" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="17" t="s">
@@ -2122,10 +2130,10 @@
       <c r="A17" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="32" t="s">
         <v>98</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -2140,33 +2148,49 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
+      <c r="H17" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M17" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N17" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O17" s="28" t="s">
+        <v>118</v>
+      </c>
       <c r="P17" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0041</v>
       </c>
       <c r="Q17" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000001000001</v>
       </c>
       <c r="R17" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000001</v>
       </c>
       <c r="S17" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T17" s="12" t="str">
         <f t="shared" ref="T17:U17" si="18">BIN2HEX(R17,2)</f>
-        <v>00</v>
+        <v>41</v>
       </c>
       <c r="U17" s="13" t="str">
         <f t="shared" si="18"/>
@@ -2198,33 +2222,49 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
+      <c r="H18" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J18" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M18" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N18" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O18" s="28" t="s">
+        <v>118</v>
+      </c>
       <c r="P18" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0041</v>
       </c>
       <c r="Q18" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000001000001</v>
       </c>
       <c r="R18" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000001</v>
       </c>
       <c r="S18" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T18" s="12" t="str">
         <f t="shared" ref="T18:U18" si="19">BIN2HEX(R18,2)</f>
-        <v>00</v>
+        <v>41</v>
       </c>
       <c r="U18" s="13" t="str">
         <f t="shared" si="19"/>
@@ -2256,33 +2296,49 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
+      <c r="H19" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M19" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N19" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O19" s="28" t="s">
+        <v>118</v>
+      </c>
       <c r="P19" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0041</v>
       </c>
       <c r="Q19" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000000001000001</v>
       </c>
       <c r="R19" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000001</v>
       </c>
       <c r="S19" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00000000</v>
       </c>
       <c r="T19" s="12" t="str">
         <f t="shared" ref="T19:U19" si="20">BIN2HEX(R19,2)</f>
-        <v>00</v>
+        <v>41</v>
       </c>
       <c r="U19" s="13" t="str">
         <f t="shared" si="20"/>
@@ -2301,7 +2357,7 @@
         <v>62</v>
       </c>
       <c r="B20" s="30"/>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="33" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="17" t="s">
@@ -2900,10 +2956,10 @@
       <c r="A28" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="32" t="s">
         <v>116</v>
       </c>
       <c r="D28" s="17" t="s">
@@ -2918,37 +2974,53 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
+      <c r="H28" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K28" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L28" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M28" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N28" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="O28" s="28" t="s">
+        <v>118</v>
+      </c>
       <c r="P28" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0842</v>
       </c>
       <c r="Q28" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100001000010</v>
       </c>
       <c r="R28" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000010</v>
       </c>
       <c r="S28" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T28" s="12" t="str">
         <f t="shared" ref="T28:U28" si="29">BIN2HEX(R28,2)</f>
-        <v>00</v>
+        <v>42</v>
       </c>
       <c r="U28" s="13" t="str">
         <f t="shared" si="29"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V28" s="12">
         <v>23</v>
@@ -2976,37 +3048,53 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
+      <c r="H29" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="J29" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K29" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L29" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M29" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N29" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="O29" s="28" t="s">
+        <v>118</v>
+      </c>
       <c r="P29" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0842</v>
       </c>
       <c r="Q29" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100001000010</v>
       </c>
       <c r="R29" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000010</v>
       </c>
       <c r="S29" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T29" s="12" t="str">
         <f t="shared" ref="T29:U29" si="30">BIN2HEX(R29,2)</f>
-        <v>00</v>
+        <v>42</v>
       </c>
       <c r="U29" s="13" t="str">
         <f t="shared" si="30"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V29" s="12">
         <v>24</v>
@@ -3034,37 +3122,53 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="H30" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I30" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="J30" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="K30" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="M30" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="N30" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="O30" s="28" t="s">
+        <v>118</v>
+      </c>
       <c r="P30" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0842</v>
       </c>
       <c r="Q30" s="12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000100001000010</v>
       </c>
       <c r="R30" s="12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>01000010</v>
       </c>
       <c r="S30" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>00001000</v>
       </c>
       <c r="T30" s="12" t="str">
         <f t="shared" ref="T30:U30" si="31">BIN2HEX(R30,2)</f>
-        <v>00</v>
+        <v>42</v>
       </c>
       <c r="U30" s="13" t="str">
         <f t="shared" si="31"/>
-        <v>00</v>
+        <v>08</v>
       </c>
       <c r="V30" s="12">
         <v>25</v>
@@ -3078,10 +3182,10 @@
       <c r="A31" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="33" t="s">
         <v>82</v>
       </c>
       <c r="D31" s="17" t="s">
@@ -3526,7 +3630,7 @@
       <c r="A37" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="31" t="s">
         <v>89</v>
       </c>
       <c r="C37" s="25" t="s">
@@ -3764,6 +3868,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="Q1:W1"/>
+    <mergeCell ref="H2:O2"/>
     <mergeCell ref="C5:C16"/>
     <mergeCell ref="B31:B36"/>
     <mergeCell ref="B37:B38"/>
@@ -3774,12 +3884,6 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="C28:C30"/>
     <mergeCell ref="C31:C36"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="H2:O2"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="A1:A2">

</xml_diff>